<commit_message>
feat: performance tuning playbook finished
</commit_message>
<xml_diff>
--- a/sql_performance_tuning/sqlserver_performance_tuning_workbook.xlsx
+++ b/sql_performance_tuning/sqlserver_performance_tuning_workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WAVES\portfolio\coding-sql\sql_performance_tuning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC37B50-8EBB-4990-9C4C-AAA658640C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C75466-563D-4595-B3E3-E99DB4D01675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-4770" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38505" yWindow="-4650" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -1481,7 +1481,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,7 +1514,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1555,8 +1555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,7 +1661,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
@@ -1990,7 +1990,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2167,7 +2169,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2320,7 +2324,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2386,7 +2392,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>193</v>
       </c>
@@ -2414,7 +2420,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>195</v>
       </c>
@@ -2442,7 +2448,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>197</v>
       </c>
@@ -2505,7 +2511,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>230</v>
       </c>
@@ -2519,7 +2525,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>231</v>
       </c>
@@ -2547,7 +2553,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>233</v>
       </c>
@@ -2589,7 +2595,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>236</v>
       </c>
@@ -2603,7 +2609,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>237</v>
       </c>
@@ -2666,7 +2672,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>269</v>
       </c>

</xml_diff>